<commit_message>
[ENH] #3070 ADd icon save in view budget_drilldown_report
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_project_base_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_project_base_report.xlsx
@@ -485,13 +485,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>